<commit_message>
Update MIGHT notebook to make it identical to YDF
</commit_message>
<xml_diff>
--- a/ydf_treeple_scaling.xlsx
+++ b/ydf_treeple_scaling.xlsx
@@ -5,17 +5,17 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ariellubonja/prog/randal_might/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://livejohnshopkins-my.sharepoint.com/personal/alubonj1_jh_edu/Documents/prog/randal_might/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{40C410D8-EB78-3D4F-8EDD-7021BCFB64B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="18" documentId="8_{40C410D8-EB78-3D4F-8EDD-7021BCFB64B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7177F523-8036-5944-94EE-3309FF1D5D08}"/>
   <bookViews>
-    <workbookView xWindow="2960" yWindow="700" windowWidth="26960" windowHeight="18660" xr2:uid="{E140FAB3-C9C6-5148-A39F-9CE8C4C5FB6E}"/>
+    <workbookView xWindow="11740" yWindow="740" windowWidth="25480" windowHeight="18660" xr2:uid="{E140FAB3-C9C6-5148-A39F-9CE8C4C5FB6E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -61,7 +61,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="167" formatCode="0.0"/>
+    <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -103,7 +103,7 @@
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -441,7 +441,7 @@
   <dimension ref="A1:J21"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A9" zoomScale="161" workbookViewId="0">
-      <selection activeCell="J13" sqref="J13"/>
+      <selection activeCell="I17" sqref="I17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -683,32 +683,80 @@
         <v>2000</v>
       </c>
       <c r="B15">
+        <v>54.9833</v>
+      </c>
+      <c r="C15">
         <v>71.569999999999993</v>
       </c>
-      <c r="C15">
+      <c r="D15">
         <v>100.58</v>
       </c>
-      <c r="D15">
+      <c r="E15">
         <v>135.66</v>
       </c>
-      <c r="E15">
+      <c r="F15">
         <v>229.83</v>
       </c>
-      <c r="F15">
+      <c r="G15">
         <v>418.77949999999998</v>
+      </c>
+      <c r="H15">
+        <v>802.49540000000002</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A16" s="1">
         <v>4000</v>
       </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B16">
+        <v>140.0341</v>
+      </c>
+      <c r="C16">
+        <v>166.26</v>
+      </c>
+      <c r="D16">
+        <v>222.1643</v>
+      </c>
+      <c r="E16">
+        <v>296.42360000000002</v>
+      </c>
+      <c r="F16">
+        <v>480.16500000000002</v>
+      </c>
+      <c r="G16">
+        <v>859.61069999999995</v>
+      </c>
+      <c r="H16">
+        <v>1610.7064</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A17" s="1">
         <v>8000</v>
       </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B17">
+        <v>341.1712</v>
+      </c>
+      <c r="C17">
+        <v>389.91930000000002</v>
+      </c>
+      <c r="D17">
+        <v>496.81790000000001</v>
+      </c>
+      <c r="E17">
+        <v>643.755</v>
+      </c>
+      <c r="F17">
+        <v>1019.6019</v>
+      </c>
+      <c r="G17">
+        <v>1776.1396999999999</v>
+      </c>
+      <c r="H17">
+        <v>3272.4283</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>4</v>
       </c>

</xml_diff>

<commit_message>
Add comment to excel results that I can't run MIGHT
</commit_message>
<xml_diff>
--- a/ydf_treeple_scaling.xlsx
+++ b/ydf_treeple_scaling.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://livejohnshopkins-my.sharepoint.com/personal/alubonj1_jh_edu/Documents/prog/randal_might/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="18" documentId="8_{40C410D8-EB78-3D4F-8EDD-7021BCFB64B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7177F523-8036-5944-94EE-3309FF1D5D08}"/>
+  <xr:revisionPtr revIDLastSave="21" documentId="8_{40C410D8-EB78-3D4F-8EDD-7021BCFB64B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E1FD934A-C70D-1F4B-A108-35F39A93872C}"/>
   <bookViews>
-    <workbookView xWindow="11740" yWindow="740" windowWidth="25480" windowHeight="18660" xr2:uid="{E140FAB3-C9C6-5148-A39F-9CE8C4C5FB6E}"/>
+    <workbookView xWindow="4440" yWindow="680" windowWidth="25480" windowHeight="18660" xr2:uid="{E140FAB3-C9C6-5148-A39F-9CE8C4C5FB6E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="7">
   <si>
     <t>n</t>
   </si>
@@ -54,6 +54,9 @@
   </si>
   <si>
     <t>nlogn</t>
+  </si>
+  <si>
+    <t>Kernel keeps restarting</t>
   </si>
 </sst>
 </file>
@@ -119,6 +122,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -438,10 +445,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB6141C5-194B-EA4E-9CBB-7FDA04883FD7}">
-  <dimension ref="A1:J21"/>
+  <dimension ref="A1:J27"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A9" zoomScale="161" workbookViewId="0">
-      <selection activeCell="I17" sqref="I17"/>
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -759,6 +766,66 @@
     <row r="21" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>4</v>
+      </c>
+      <c r="B21" t="s">
+        <v>1</v>
+      </c>
+      <c r="C21" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>0</v>
+      </c>
+      <c r="B22" s="1">
+        <v>160</v>
+      </c>
+      <c r="C22" s="1">
+        <v>320</v>
+      </c>
+      <c r="D22" s="1">
+        <v>640</v>
+      </c>
+      <c r="E22" s="1">
+        <v>1024</v>
+      </c>
+      <c r="F22" s="1">
+        <v>2048</v>
+      </c>
+      <c r="G22" s="1">
+        <v>4096</v>
+      </c>
+      <c r="H22" s="1">
+        <v>8192</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A23" s="1">
+        <v>500</v>
+      </c>
+      <c r="B23" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A24" s="1">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A25" s="1">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A26" s="1">
+        <v>4000</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A27" s="1">
+        <v>8000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add sparse_oblique_exponent to YDF. Add more d values to MIGHT experiments. Update XLSX
</commit_message>
<xml_diff>
--- a/ydf_treeple_scaling.xlsx
+++ b/ydf_treeple_scaling.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://livejohnshopkins-my.sharepoint.com/personal/alubonj1_jh_edu/Documents/prog/randal_might/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="21" documentId="8_{40C410D8-EB78-3D4F-8EDD-7021BCFB64B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E1FD934A-C70D-1F4B-A108-35F39A93872C}"/>
+  <xr:revisionPtr revIDLastSave="108" documentId="8_{40C410D8-EB78-3D4F-8EDD-7021BCFB64B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5BE97296-079E-2545-9D8B-0F35684AF0BD}"/>
   <bookViews>
-    <workbookView xWindow="4440" yWindow="680" windowWidth="25480" windowHeight="18660" xr2:uid="{E140FAB3-C9C6-5148-A39F-9CE8C4C5FB6E}"/>
+    <workbookView xWindow="10680" yWindow="1600" windowWidth="25480" windowHeight="18660" xr2:uid="{E140FAB3-C9C6-5148-A39F-9CE8C4C5FB6E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="11">
   <si>
     <t>n</t>
   </si>
@@ -56,7 +56,19 @@
     <t>nlogn</t>
   </si>
   <si>
-    <t>Kernel keeps restarting</t>
+    <t>3 repeats</t>
+  </si>
+  <si>
+    <t>0 repeats</t>
+  </si>
+  <si>
+    <t>m5.metal</t>
+  </si>
+  <si>
+    <t>double-check work of YDF</t>
+  </si>
+  <si>
+    <t>YDF - sparse_oblique_exponent = 1</t>
   </si>
 </sst>
 </file>
@@ -66,7 +78,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -79,6 +91,13 @@
       <i/>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="12"/>
       <name val="Aptos Narrow"/>
       <scheme val="minor"/>
     </font>
@@ -103,10 +122,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -445,10 +465,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB6141C5-194B-EA4E-9CBB-7FDA04883FD7}">
-  <dimension ref="A1:J27"/>
+  <dimension ref="A1:L36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="161" workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="118" workbookViewId="0">
+      <selection activeCell="L31" sqref="L31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -589,6 +609,11 @@
       <c r="G7" s="2"/>
       <c r="H7" s="2"/>
     </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B9" t="s">
+        <v>8</v>
+      </c>
+    </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>3</v>
@@ -599,6 +624,9 @@
       <c r="C11" t="s">
         <v>2</v>
       </c>
+      <c r="E11" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
@@ -737,7 +765,7 @@
         <v>1610.7064</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A17" s="1">
         <v>8000</v>
       </c>
@@ -763,9 +791,19 @@
         <v>3272.4283</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="I19" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B21" t="s">
         <v>1</v>
@@ -773,8 +811,11 @@
       <c r="C21" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="E21" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>0</v>
       </c>
@@ -800,36 +841,321 @@
         <v>8192</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A23" s="1">
         <v>500</v>
       </c>
-      <c r="B23" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B23">
+        <v>0.39350000000000002</v>
+      </c>
+      <c r="C23">
+        <v>0.96799999999999997</v>
+      </c>
+      <c r="D23">
+        <v>2.7608999999999999</v>
+      </c>
+      <c r="E23">
+        <v>6.0873999999999997</v>
+      </c>
+      <c r="F23">
+        <v>20.634899999999998</v>
+      </c>
+      <c r="G23">
+        <v>73.389200000000002</v>
+      </c>
+      <c r="H23">
+        <v>203.8382</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A24" s="1">
         <v>1000</v>
       </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B24">
+        <v>0.87629999999999997</v>
+      </c>
+      <c r="C24">
+        <v>2.1465999999999998</v>
+      </c>
+      <c r="D24">
+        <v>5.9234999999999998</v>
+      </c>
+      <c r="E24">
+        <v>12.6541</v>
+      </c>
+      <c r="F24">
+        <v>41.807000000000002</v>
+      </c>
+      <c r="G24">
+        <v>146.67509999999999</v>
+      </c>
+      <c r="H24">
+        <v>399.89870000000002</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A25" s="1">
         <v>2000</v>
       </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B25">
+        <v>2.0815999999999999</v>
+      </c>
+      <c r="C25">
+        <v>4.9962999999999997</v>
+      </c>
+      <c r="D25">
+        <v>12.973000000000001</v>
+      </c>
+      <c r="E25">
+        <v>26.984400000000001</v>
+      </c>
+      <c r="F25">
+        <v>85.486599999999996</v>
+      </c>
+      <c r="G25">
+        <v>295.16609999999997</v>
+      </c>
+      <c r="H25">
+        <v>802.49540000000002</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A26" s="1">
         <v>4000</v>
       </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B26">
+        <v>140.0341</v>
+      </c>
+      <c r="C26">
+        <v>166.26</v>
+      </c>
+      <c r="D26">
+        <v>222.1643</v>
+      </c>
+      <c r="E26">
+        <v>296.42360000000002</v>
+      </c>
+      <c r="F26">
+        <v>480.16500000000002</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A27" s="1">
         <v>8000</v>
       </c>
     </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>4</v>
+      </c>
+      <c r="B30" t="s">
+        <v>1</v>
+      </c>
+      <c r="C30" t="s">
+        <v>2</v>
+      </c>
+      <c r="E30" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>0</v>
+      </c>
+      <c r="B31" s="1">
+        <v>160</v>
+      </c>
+      <c r="C31" s="1">
+        <v>320</v>
+      </c>
+      <c r="D31" s="1">
+        <v>640</v>
+      </c>
+      <c r="E31" s="1">
+        <v>1024</v>
+      </c>
+      <c r="F31" s="1">
+        <v>2048</v>
+      </c>
+      <c r="G31" s="1">
+        <v>4096</v>
+      </c>
+      <c r="H31" s="1">
+        <v>8192</v>
+      </c>
+      <c r="I31" s="3">
+        <f>8192*2</f>
+        <v>16384</v>
+      </c>
+      <c r="J31" s="1">
+        <f>I31*2</f>
+        <v>32768</v>
+      </c>
+      <c r="K31" s="1">
+        <f t="shared" ref="K31:L31" si="0">J31*2</f>
+        <v>65536</v>
+      </c>
+      <c r="L31" s="1">
+        <f t="shared" si="0"/>
+        <v>131072</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A32" s="1">
+        <v>500</v>
+      </c>
+      <c r="B32">
+        <v>7.1136999999999997</v>
+      </c>
+      <c r="C32">
+        <v>7.2495000000000003</v>
+      </c>
+      <c r="D32">
+        <v>7.4531999999999998</v>
+      </c>
+      <c r="E32">
+        <v>7.5956999999999999</v>
+      </c>
+      <c r="F32">
+        <v>8.0981000000000005</v>
+      </c>
+      <c r="G32">
+        <v>10.3894</v>
+      </c>
+      <c r="H32">
+        <v>20.5901</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A33" s="1">
+        <v>1000</v>
+      </c>
+      <c r="B33">
+        <v>10.1264</v>
+      </c>
+      <c r="C33">
+        <v>10.262</v>
+      </c>
+      <c r="D33">
+        <v>10.4505</v>
+      </c>
+      <c r="E33">
+        <v>10.7079</v>
+      </c>
+      <c r="F33">
+        <v>11.536300000000001</v>
+      </c>
+      <c r="G33">
+        <v>16.9053</v>
+      </c>
+      <c r="H33">
+        <v>38.569699999999997</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A34" s="1">
+        <v>2000</v>
+      </c>
+      <c r="B34">
+        <v>15.675000000000001</v>
+      </c>
+      <c r="C34">
+        <v>15.718</v>
+      </c>
+      <c r="D34">
+        <v>16.107099999999999</v>
+      </c>
+      <c r="E34">
+        <v>16.459499999999998</v>
+      </c>
+      <c r="F34">
+        <v>18.554200000000002</v>
+      </c>
+      <c r="G34">
+        <v>32.394399999999997</v>
+      </c>
+      <c r="H34">
+        <v>76.351500000000001</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A35" s="1">
+        <v>4000</v>
+      </c>
+      <c r="B35">
+        <v>25.873999999999999</v>
+      </c>
+      <c r="C35">
+        <v>26.148499999999999</v>
+      </c>
+      <c r="D35">
+        <v>26.886099999999999</v>
+      </c>
+      <c r="E35">
+        <v>27.731300000000001</v>
+      </c>
+      <c r="F35">
+        <v>31.893699999999999</v>
+      </c>
+      <c r="G35">
+        <v>64.934200000000004</v>
+      </c>
+      <c r="H35">
+        <v>160.38890000000001</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A36" s="1">
+        <v>8000</v>
+      </c>
+      <c r="B36">
+        <v>45.749000000000002</v>
+      </c>
+      <c r="C36">
+        <v>46.4161</v>
+      </c>
+      <c r="D36">
+        <v>48.104799999999997</v>
+      </c>
+      <c r="E36">
+        <v>50.235599999999998</v>
+      </c>
+      <c r="F36">
+        <v>59.738900000000001</v>
+      </c>
+      <c r="G36">
+        <v>132.6771</v>
+      </c>
+      <c r="H36">
+        <v>307.22840000000002</v>
+      </c>
+    </row>
   </sheetData>
   <conditionalFormatting sqref="B3:H7">
+    <cfRule type="colorScale" priority="4">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B13:H17">
+    <cfRule type="colorScale" priority="3">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B32:H36">
     <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="min"/>
@@ -841,7 +1167,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B13:H17">
+  <conditionalFormatting sqref="B23:H27">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>

</xml_diff>

<commit_message>
TODO need to fix Treeple inference code - it's per tree
</commit_message>
<xml_diff>
--- a/ydf_treeple_scaling.xlsx
+++ b/ydf_treeple_scaling.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://livejohnshopkins-my.sharepoint.com/personal/alubonj1_jh_edu/Documents/prog/randal_might/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="255" documentId="8_{40C410D8-EB78-3D4F-8EDD-7021BCFB64B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D38A6B7D-32A3-4C43-B178-0D31FD9A59E8}"/>
+  <xr:revisionPtr revIDLastSave="468" documentId="8_{40C410D8-EB78-3D4F-8EDD-7021BCFB64B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7CA645D0-5055-C546-8F7A-2C70630B9718}"/>
   <bookViews>
-    <workbookView xWindow="12380" yWindow="1040" windowWidth="16520" windowHeight="18660" xr2:uid="{E140FAB3-C9C6-5148-A39F-9CE8C4C5FB6E}"/>
+    <workbookView xWindow="11100" yWindow="680" windowWidth="17540" windowHeight="18660" xr2:uid="{E140FAB3-C9C6-5148-A39F-9CE8C4C5FB6E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="16">
   <si>
     <t>n</t>
   </si>
@@ -79,6 +79,12 @@
   <si>
     <t>keeping n_attributes = 128</t>
   </si>
+  <si>
+    <t>size in MB</t>
+  </si>
+  <si>
+    <t>WRONG code used for Treeple inference!</t>
+  </si>
 </sst>
 </file>
 
@@ -87,7 +93,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -117,6 +123,13 @@
       <name val="Aptos Narrow"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color theme="2"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -138,12 +151,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -482,10 +496,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB6141C5-194B-EA4E-9CBB-7FDA04883FD7}">
-  <dimension ref="A1:AA42"/>
+  <dimension ref="A1:AA50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="S18" zoomScale="118" workbookViewId="0">
-      <selection activeCell="AA36" sqref="AA36"/>
+    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="118" workbookViewId="0">
+      <selection activeCell="P44" sqref="P44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -814,7 +828,7 @@
       </c>
     </row>
     <row r="19" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="I19" t="s">
+      <c r="I19" s="4" t="s">
         <v>9</v>
       </c>
     </row>
@@ -822,6 +836,9 @@
       <c r="A20" t="s">
         <v>10</v>
       </c>
+      <c r="P20" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="21" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
@@ -831,10 +848,22 @@
         <v>1</v>
       </c>
       <c r="C21" t="s">
+        <v>13</v>
+      </c>
+      <c r="E21" t="s">
+        <v>6</v>
+      </c>
+      <c r="P21" t="s">
+        <v>3</v>
+      </c>
+      <c r="Q21" t="s">
+        <v>1</v>
+      </c>
+      <c r="R21" t="s">
         <v>2</v>
       </c>
-      <c r="E21" t="s">
-        <v>7</v>
+      <c r="T21" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="22" spans="1:27" x14ac:dyDescent="0.2">
@@ -842,13 +871,13 @@
         <v>0</v>
       </c>
       <c r="B22" s="1">
-        <v>160</v>
+        <v>128</v>
       </c>
       <c r="C22" s="1">
-        <v>320</v>
+        <v>256</v>
       </c>
       <c r="D22" s="1">
-        <v>640</v>
+        <v>512</v>
       </c>
       <c r="E22" s="1">
         <v>1024</v>
@@ -862,637 +891,1293 @@
       <c r="H22" s="1">
         <v>8192</v>
       </c>
+      <c r="I22" s="3">
+        <f>8192*2</f>
+        <v>16384</v>
+      </c>
+      <c r="J22" s="1">
+        <f>I22*2</f>
+        <v>32768</v>
+      </c>
+      <c r="K22" s="1">
+        <f t="shared" ref="K22" si="0">J22*2</f>
+        <v>65536</v>
+      </c>
+      <c r="L22" s="1">
+        <f t="shared" ref="L22" si="1">K22*2</f>
+        <v>131072</v>
+      </c>
+      <c r="P22" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q22" s="1">
+        <v>128</v>
+      </c>
+      <c r="R22" s="1">
+        <v>256</v>
+      </c>
+      <c r="S22" s="1">
+        <v>512</v>
+      </c>
+      <c r="T22" s="1">
+        <v>1024</v>
+      </c>
+      <c r="U22" s="1">
+        <v>2048</v>
+      </c>
+      <c r="V22" s="1">
+        <v>4096</v>
+      </c>
+      <c r="W22" s="1">
+        <v>8192</v>
+      </c>
+      <c r="X22" s="3">
+        <f>8192*2</f>
+        <v>16384</v>
+      </c>
+      <c r="Y22" s="1">
+        <f>X22*2</f>
+        <v>32768</v>
+      </c>
+      <c r="Z22" s="1">
+        <f t="shared" ref="Z22" si="2">Y22*2</f>
+        <v>65536</v>
+      </c>
+      <c r="AA22" s="1">
+        <f t="shared" ref="AA22" si="3">Z22*2</f>
+        <v>131072</v>
+      </c>
     </row>
     <row r="23" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A23" s="1">
-        <v>500</v>
+        <v>128</v>
       </c>
       <c r="B23">
-        <v>0.39350000000000002</v>
+        <v>7.2599999999999998E-2</v>
       </c>
       <c r="C23">
-        <v>0.96799999999999997</v>
+        <v>0.17219999999999999</v>
       </c>
       <c r="D23">
-        <v>2.7608999999999999</v>
+        <v>0.5212</v>
       </c>
       <c r="E23">
-        <v>6.0873999999999997</v>
+        <v>1.6742999999999999</v>
       </c>
       <c r="F23">
-        <v>20.634899999999998</v>
+        <v>5.8550000000000004</v>
       </c>
       <c r="G23">
-        <v>73.389200000000002</v>
+        <v>21.836300000000001</v>
       </c>
       <c r="H23">
-        <v>203.8382</v>
+        <v>61.622399999999999</v>
+      </c>
+      <c r="I23">
+        <v>122.895</v>
+      </c>
+      <c r="J23">
+        <v>248.9051</v>
+      </c>
+      <c r="K23">
+        <v>501.2328</v>
+      </c>
+      <c r="L23">
+        <v>1040.9502</v>
+      </c>
+      <c r="P23" s="1">
+        <v>128</v>
+      </c>
+      <c r="Q23">
+        <v>1.04E-2</v>
+      </c>
+      <c r="R23">
+        <v>1.5699999999999999E-2</v>
+      </c>
+      <c r="S23">
+        <v>2.58E-2</v>
+      </c>
+      <c r="T23">
+        <v>4.6199999999999998E-2</v>
+      </c>
+      <c r="U23">
+        <v>0.12939999999999999</v>
+      </c>
+      <c r="V23">
+        <v>0.2414</v>
+      </c>
+      <c r="W23">
+        <v>0.432</v>
+      </c>
+      <c r="X23">
+        <v>0.91139999999999999</v>
+      </c>
+      <c r="Y23">
+        <v>1.7851999999999999</v>
+      </c>
+      <c r="Z23">
+        <v>3.4790000000000001</v>
+      </c>
+      <c r="AA23">
+        <v>7.5664999999999996</v>
       </c>
     </row>
     <row r="24" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A24" s="1">
-        <v>1000</v>
+        <v>256</v>
       </c>
       <c r="B24">
-        <v>0.87629999999999997</v>
+        <v>0.16819999999999999</v>
       </c>
       <c r="C24">
-        <v>2.1465999999999998</v>
+        <v>0.33650000000000002</v>
       </c>
       <c r="D24">
-        <v>5.9234999999999998</v>
+        <v>0.97</v>
       </c>
       <c r="E24">
-        <v>12.6541</v>
+        <v>3.1377000000000002</v>
       </c>
       <c r="F24">
-        <v>41.807000000000002</v>
+        <v>10.8523</v>
       </c>
       <c r="G24">
-        <v>146.67509999999999</v>
+        <v>39.637999999999998</v>
       </c>
       <c r="H24">
-        <v>399.89870000000002</v>
+        <v>110.7223</v>
+      </c>
+      <c r="I24">
+        <v>219.44309999999999</v>
+      </c>
+      <c r="J24">
+        <v>437.9803</v>
+      </c>
+      <c r="K24">
+        <v>880.21349999999995</v>
+      </c>
+      <c r="L24">
+        <v>1788.5415</v>
+      </c>
+      <c r="P24" s="1">
+        <v>256</v>
+      </c>
+      <c r="Q24">
+        <v>1.6400000000000001E-2</v>
+      </c>
+      <c r="R24">
+        <v>2.0799999999999999E-2</v>
+      </c>
+      <c r="S24">
+        <v>3.1699999999999999E-2</v>
+      </c>
+      <c r="T24">
+        <v>7.1400000000000005E-2</v>
+      </c>
+      <c r="U24">
+        <v>0.1166</v>
+      </c>
+      <c r="V24">
+        <v>0.2303</v>
+      </c>
+      <c r="W24">
+        <v>0.44069999999999998</v>
+      </c>
+      <c r="X24">
+        <v>0.87970000000000004</v>
+      </c>
+      <c r="Y24">
+        <v>1.8123</v>
+      </c>
+      <c r="Z24">
+        <v>3.5550999999999999</v>
+      </c>
+      <c r="AA24">
+        <v>7.3433999999999999</v>
       </c>
     </row>
     <row r="25" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A25" s="1">
-        <v>2000</v>
+        <v>512</v>
       </c>
       <c r="B25">
-        <v>2.0815999999999999</v>
+        <v>0.3301</v>
       </c>
       <c r="C25">
-        <v>4.9962999999999997</v>
+        <v>0.73140000000000005</v>
       </c>
       <c r="D25">
-        <v>12.973000000000001</v>
+        <v>2.0118</v>
       </c>
       <c r="E25">
-        <v>26.984400000000001</v>
+        <v>6.2449000000000003</v>
       </c>
       <c r="F25">
-        <v>85.486599999999996</v>
+        <v>21.007400000000001</v>
       </c>
       <c r="G25">
-        <v>295.16609999999997</v>
+        <v>75.665000000000006</v>
       </c>
       <c r="H25">
-        <v>802.49540000000002</v>
+        <v>209.00059999999999</v>
+      </c>
+      <c r="I25">
+        <v>411.36149999999998</v>
+      </c>
+      <c r="J25">
+        <v>820.17280000000005</v>
+      </c>
+      <c r="K25">
+        <v>1639.5507</v>
+      </c>
+      <c r="L25">
+        <v>3330.5740000000001</v>
+      </c>
+      <c r="P25" s="1">
+        <v>512</v>
+      </c>
+      <c r="Q25">
+        <v>2.5700000000000001E-2</v>
+      </c>
+      <c r="R25">
+        <v>2.8400000000000002E-2</v>
+      </c>
+      <c r="S25">
+        <v>4.0500000000000001E-2</v>
+      </c>
+      <c r="T25">
+        <v>5.91E-2</v>
+      </c>
+      <c r="U25">
+        <v>0.12939999999999999</v>
+      </c>
+      <c r="V25">
+        <v>0.26429999999999998</v>
+      </c>
+      <c r="W25">
+        <v>0.46310000000000001</v>
+      </c>
+      <c r="X25">
+        <v>0.90900000000000003</v>
+      </c>
+      <c r="Y25">
+        <v>1.8573999999999999</v>
+      </c>
+      <c r="Z25">
+        <v>3.5846</v>
+      </c>
+      <c r="AA25">
+        <v>7.8289999999999997</v>
       </c>
     </row>
     <row r="26" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A26" s="1">
-        <v>4000</v>
+        <v>1024</v>
       </c>
       <c r="B26">
-        <v>140.0341</v>
+        <v>0.74029999999999996</v>
       </c>
       <c r="C26">
-        <v>166.26</v>
+        <v>1.6416999999999999</v>
       </c>
       <c r="D26">
-        <v>222.1643</v>
+        <v>4.3486000000000002</v>
       </c>
       <c r="E26">
-        <v>296.42360000000002</v>
+        <v>12.9138</v>
       </c>
       <c r="F26">
-        <v>480.16500000000002</v>
+        <v>42.607999999999997</v>
+      </c>
+      <c r="G26">
+        <v>149.8098</v>
+      </c>
+      <c r="H26">
+        <v>409.59140000000002</v>
+      </c>
+      <c r="I26">
+        <v>800.21600000000001</v>
+      </c>
+      <c r="J26">
+        <v>1586.1370999999999</v>
+      </c>
+      <c r="K26">
+        <v>3175.3227999999999</v>
+      </c>
+      <c r="L26">
+        <v>6380.7353999999996</v>
+      </c>
+      <c r="P26" s="1">
+        <v>1024</v>
+      </c>
+      <c r="Q26">
+        <v>3.9899999999999998E-2</v>
+      </c>
+      <c r="R26">
+        <v>4.8500000000000001E-2</v>
+      </c>
+      <c r="S26">
+        <v>5.2400000000000002E-2</v>
+      </c>
+      <c r="T26">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="U26">
+        <v>0.12859999999999999</v>
+      </c>
+      <c r="V26">
+        <v>0.2402</v>
+      </c>
+      <c r="W26">
+        <v>0.54090000000000005</v>
+      </c>
+      <c r="X26">
+        <v>0.97450000000000003</v>
+      </c>
+      <c r="Y26">
+        <v>1.9245000000000001</v>
+      </c>
+      <c r="Z26">
+        <v>4.0541999999999998</v>
+      </c>
+      <c r="AA26">
+        <v>7.9656000000000002</v>
       </c>
     </row>
     <row r="27" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A27" s="1">
-        <v>8000</v>
+        <v>2048</v>
+      </c>
+      <c r="B27">
+        <v>1.7276</v>
+      </c>
+      <c r="C27">
+        <v>3.8426999999999998</v>
+      </c>
+      <c r="D27">
+        <v>9.6146999999999991</v>
+      </c>
+      <c r="E27">
+        <v>27.493099999999998</v>
+      </c>
+      <c r="F27">
+        <v>87.789299999999997</v>
+      </c>
+      <c r="G27">
+        <v>301.5292</v>
+      </c>
+      <c r="H27">
+        <v>817.23440000000005</v>
+      </c>
+      <c r="I27">
+        <v>1587.682</v>
+      </c>
+      <c r="J27">
+        <v>3134.7370999999998</v>
+      </c>
+      <c r="P27" s="1">
+        <v>2048</v>
+      </c>
+      <c r="Q27">
+        <v>7.7700000000000005E-2</v>
+      </c>
+      <c r="R27">
+        <v>7.8299999999999995E-2</v>
+      </c>
+      <c r="S27">
+        <v>9.5500000000000002E-2</v>
+      </c>
+      <c r="T27">
+        <v>0.11020000000000001</v>
+      </c>
+      <c r="U27">
+        <v>0.17979999999999999</v>
+      </c>
+      <c r="V27">
+        <v>0.31419999999999998</v>
+      </c>
+      <c r="W27">
+        <v>0.60670000000000002</v>
+      </c>
+      <c r="X27">
+        <v>1.1544000000000001</v>
+      </c>
+      <c r="Y27">
+        <v>2.0686</v>
+      </c>
+    </row>
+    <row r="28" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A28" s="1">
+        <v>4096</v>
+      </c>
+      <c r="P28" s="1">
+        <v>4096</v>
       </c>
     </row>
     <row r="29" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="P29" t="s">
+      <c r="A29" s="1">
+        <v>8192</v>
+      </c>
+      <c r="P29" s="1">
+        <v>8192</v>
+      </c>
+    </row>
+    <row r="30" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A30" s="1">
+        <v>16384</v>
+      </c>
+      <c r="P30" s="1">
+        <v>16384</v>
+      </c>
+    </row>
+    <row r="31" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A31" s="1">
+        <v>32768</v>
+      </c>
+      <c r="P31" s="1">
+        <v>32768</v>
+      </c>
+    </row>
+    <row r="32" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A32" s="1">
+        <v>65536</v>
+      </c>
+      <c r="P32" s="1">
+        <v>65536</v>
+      </c>
+    </row>
+    <row r="33" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A33" s="1">
+        <v>131072</v>
+      </c>
+      <c r="P33" s="1">
+        <v>131072</v>
+      </c>
+    </row>
+    <row r="35" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="K35" t="s">
+        <v>14</v>
+      </c>
+      <c r="P35" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="30" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="A30" t="s">
+    <row r="36" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
         <v>4</v>
       </c>
-      <c r="B30" t="s">
+      <c r="B36" t="s">
         <v>1</v>
       </c>
-      <c r="C30" t="s">
+      <c r="C36" t="s">
         <v>13</v>
       </c>
-      <c r="E30" t="s">
+      <c r="E36" t="s">
         <v>6</v>
       </c>
-      <c r="P30" t="s">
+      <c r="P36" t="s">
         <v>4</v>
       </c>
-      <c r="Q30" t="s">
+      <c r="Q36" t="s">
         <v>1</v>
       </c>
-      <c r="R30" t="s">
+      <c r="R36" t="s">
         <v>2</v>
       </c>
-      <c r="T30" t="s">
+      <c r="T36" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="31" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="A31" t="s">
+    <row r="37" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
         <v>0</v>
       </c>
-      <c r="B31" s="1">
+      <c r="B37" s="1">
         <v>128</v>
       </c>
-      <c r="C31" s="1">
+      <c r="C37" s="1">
         <v>256</v>
       </c>
-      <c r="D31" s="1">
+      <c r="D37" s="1">
         <v>512</v>
       </c>
-      <c r="E31" s="1">
+      <c r="E37" s="1">
         <v>1024</v>
       </c>
-      <c r="F31" s="1">
+      <c r="F37" s="1">
         <v>2048</v>
       </c>
-      <c r="G31" s="1">
+      <c r="G37" s="1">
         <v>4096</v>
       </c>
-      <c r="H31" s="1">
+      <c r="H37" s="1">
         <v>8192</v>
       </c>
-      <c r="I31" s="3">
+      <c r="I37" s="3">
         <f>8192*2</f>
         <v>16384</v>
       </c>
-      <c r="J31" s="1">
-        <f>I31*2</f>
+      <c r="J37" s="1">
+        <f>I37*2</f>
         <v>32768</v>
       </c>
-      <c r="K31" s="1">
-        <f t="shared" ref="K31:L31" si="0">J31*2</f>
+      <c r="K37" s="1">
+        <f t="shared" ref="K37:L37" si="4">J37*2</f>
         <v>65536</v>
       </c>
-      <c r="L31" s="1">
-        <f t="shared" si="0"/>
+      <c r="L37" s="1">
+        <f t="shared" si="4"/>
         <v>131072</v>
       </c>
-      <c r="P31" t="s">
+      <c r="P37" t="s">
         <v>0</v>
       </c>
-      <c r="Q31" s="1">
+      <c r="Q37" s="1">
         <v>128</v>
       </c>
-      <c r="R31" s="1">
+      <c r="R37" s="1">
         <v>256</v>
       </c>
-      <c r="S31" s="1">
+      <c r="S37" s="1">
         <v>512</v>
       </c>
-      <c r="T31" s="1">
+      <c r="T37" s="1">
         <v>1024</v>
       </c>
-      <c r="U31" s="1">
+      <c r="U37" s="1">
         <v>2048</v>
       </c>
-      <c r="V31" s="1">
+      <c r="V37" s="1">
         <v>4096</v>
       </c>
-      <c r="W31" s="1">
+      <c r="W37" s="1">
         <v>8192</v>
       </c>
-      <c r="X31" s="3">
+      <c r="X37" s="3">
         <f>8192*2</f>
         <v>16384</v>
       </c>
-      <c r="Y31" s="1">
-        <f>X31*2</f>
+      <c r="Y37" s="1">
+        <f>X37*2</f>
         <v>32768</v>
       </c>
-      <c r="Z31" s="1">
-        <f t="shared" ref="Z31" si="1">Y31*2</f>
+      <c r="Z37" s="1">
+        <f t="shared" ref="Z37" si="5">Y37*2</f>
         <v>65536</v>
       </c>
-      <c r="AA31" s="1">
-        <f t="shared" ref="AA31" si="2">Z31*2</f>
+      <c r="AA37" s="1">
+        <f t="shared" ref="AA37" si="6">Z37*2</f>
         <v>131072</v>
-      </c>
-    </row>
-    <row r="32" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="A32" s="1">
-        <v>128</v>
-      </c>
-      <c r="B32">
-        <v>4.8661000000000003</v>
-      </c>
-      <c r="C32">
-        <v>4.8882000000000003</v>
-      </c>
-      <c r="D32">
-        <v>4.9641000000000002</v>
-      </c>
-      <c r="E32">
-        <v>5.1196000000000002</v>
-      </c>
-      <c r="F32">
-        <v>5.3280000000000003</v>
-      </c>
-      <c r="G32">
-        <v>5.6430999999999996</v>
-      </c>
-      <c r="H32">
-        <v>6.6346999999999996</v>
-      </c>
-      <c r="I32">
-        <v>9.8186999999999998</v>
-      </c>
-      <c r="J32">
-        <v>17.505199999999999</v>
-      </c>
-      <c r="K32">
-        <v>35.870100000000001</v>
-      </c>
-      <c r="L32">
-        <v>74.410600000000002</v>
-      </c>
-      <c r="P32" s="1">
-        <v>128</v>
-      </c>
-      <c r="Q32">
-        <v>1.0468</v>
-      </c>
-      <c r="R32">
-        <v>1.4205000000000001</v>
-      </c>
-      <c r="S32">
-        <v>2.2820999999999998</v>
-      </c>
-      <c r="T32">
-        <v>3.9356</v>
-      </c>
-      <c r="U32">
-        <v>7.2767999999999997</v>
-      </c>
-      <c r="V32">
-        <v>13.8726</v>
-      </c>
-      <c r="W32">
-        <v>27.044</v>
-      </c>
-      <c r="X32">
-        <v>53.479799999999997</v>
-      </c>
-      <c r="Y32">
-        <v>106.0325</v>
-      </c>
-      <c r="Z32">
-        <v>211.68559999999999</v>
-      </c>
-      <c r="AA32">
-        <v>423.58030000000002</v>
-      </c>
-    </row>
-    <row r="33" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="A33" s="1">
-        <v>256</v>
-      </c>
-      <c r="B33">
-        <v>5.7586000000000004</v>
-      </c>
-      <c r="C33">
-        <v>5.8208000000000002</v>
-      </c>
-      <c r="D33">
-        <v>5.9991000000000003</v>
-      </c>
-      <c r="E33">
-        <v>6.0632999999999999</v>
-      </c>
-      <c r="F33">
-        <v>6.3122999999999996</v>
-      </c>
-      <c r="G33">
-        <v>6.9637000000000002</v>
-      </c>
-      <c r="H33">
-        <v>9.3026</v>
-      </c>
-      <c r="I33">
-        <v>17.875800000000002</v>
-      </c>
-      <c r="J33">
-        <v>33.2316</v>
-      </c>
-      <c r="K33">
-        <v>69.363399999999999</v>
-      </c>
-      <c r="L33">
-        <v>145.5532</v>
-      </c>
-      <c r="P33" s="1">
-        <v>256</v>
-      </c>
-      <c r="Q33">
-        <v>1.0177</v>
-      </c>
-      <c r="R33">
-        <v>1.4511000000000001</v>
-      </c>
-      <c r="S33">
-        <v>2.3130999999999999</v>
-      </c>
-      <c r="T33">
-        <v>3.9988000000000001</v>
-      </c>
-      <c r="U33">
-        <v>7.3720999999999997</v>
-      </c>
-      <c r="V33">
-        <v>14.101900000000001</v>
-      </c>
-      <c r="W33">
-        <v>27.500599999999999</v>
-      </c>
-      <c r="X33">
-        <v>54.220500000000001</v>
-      </c>
-      <c r="Y33">
-        <v>107.7698</v>
-      </c>
-      <c r="Z33">
-        <v>216.90170000000001</v>
-      </c>
-      <c r="AA33">
-        <v>442.46089999999998</v>
-      </c>
-    </row>
-    <row r="34" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="A34" s="1">
-        <v>512</v>
-      </c>
-      <c r="B34">
-        <v>7.2171000000000003</v>
-      </c>
-      <c r="C34">
-        <v>7.2676999999999996</v>
-      </c>
-      <c r="D34">
-        <v>7.4058000000000002</v>
-      </c>
-      <c r="E34">
-        <v>7.6805000000000003</v>
-      </c>
-      <c r="F34">
-        <v>7.8780000000000001</v>
-      </c>
-      <c r="G34">
-        <v>9.2751999999999999</v>
-      </c>
-      <c r="H34">
-        <v>16.802900000000001</v>
-      </c>
-      <c r="I34">
-        <v>36.252899999999997</v>
-      </c>
-      <c r="J34">
-        <v>64.372200000000007</v>
-      </c>
-      <c r="K34">
-        <v>136.39420000000001</v>
-      </c>
-      <c r="L34">
-        <v>283.41660000000002</v>
-      </c>
-      <c r="P34" s="1">
-        <v>512</v>
-      </c>
-      <c r="Q34">
-        <v>1.0412999999999999</v>
-      </c>
-      <c r="R34">
-        <v>1.4725999999999999</v>
-      </c>
-      <c r="S34">
-        <v>2.3595000000000002</v>
-      </c>
-      <c r="T34">
-        <v>4.0561999999999996</v>
-      </c>
-      <c r="U34">
-        <v>7.4831000000000003</v>
-      </c>
-      <c r="V34">
-        <v>14.2651</v>
-      </c>
-      <c r="W34">
-        <v>27.85</v>
-      </c>
-      <c r="X34">
-        <v>55.3964</v>
-      </c>
-      <c r="Y34">
-        <v>111.3929</v>
-      </c>
-      <c r="Z34">
-        <v>230.0112</v>
-      </c>
-      <c r="AA34">
-        <v>462.54090000000002</v>
-      </c>
-    </row>
-    <row r="35" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="A35" s="1">
-        <v>1024</v>
-      </c>
-      <c r="B35">
-        <v>10.410600000000001</v>
-      </c>
-      <c r="C35">
-        <v>10.4734</v>
-      </c>
-      <c r="D35">
-        <v>10.660299999999999</v>
-      </c>
-      <c r="E35">
-        <v>10.9011</v>
-      </c>
-      <c r="F35">
-        <v>11.475300000000001</v>
-      </c>
-      <c r="G35">
-        <v>14.431100000000001</v>
-      </c>
-      <c r="H35">
-        <v>31.186900000000001</v>
-      </c>
-      <c r="I35">
-        <v>69.664000000000001</v>
-      </c>
-      <c r="J35">
-        <v>129.32140000000001</v>
-      </c>
-      <c r="K35">
-        <v>277.1678</v>
-      </c>
-      <c r="L35">
-        <v>570.41139999999996</v>
-      </c>
-      <c r="P35" s="1">
-        <v>1024</v>
-      </c>
-      <c r="Q35">
-        <v>1.0940000000000001</v>
-      </c>
-      <c r="R35">
-        <v>1.5558000000000001</v>
-      </c>
-      <c r="S35">
-        <v>2.4428000000000001</v>
-      </c>
-      <c r="T35">
-        <v>4.2047999999999996</v>
-      </c>
-      <c r="U35">
-        <v>7.7328000000000001</v>
-      </c>
-      <c r="V35">
-        <v>14.768000000000001</v>
-      </c>
-      <c r="W35">
-        <v>29.1662</v>
-      </c>
-      <c r="X35">
-        <v>58.742699999999999</v>
-      </c>
-      <c r="Y35">
-        <v>124.4648</v>
-      </c>
-      <c r="Z35">
-        <v>249.95740000000001</v>
-      </c>
-      <c r="AA35">
-        <v>499.8057</v>
-      </c>
-    </row>
-    <row r="36" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="A36" s="1">
-        <v>2048</v>
-      </c>
-      <c r="B36">
-        <v>15.927099999999999</v>
-      </c>
-      <c r="C36">
-        <v>16.150400000000001</v>
-      </c>
-      <c r="D36">
-        <v>16.379100000000001</v>
-      </c>
-      <c r="E36">
-        <v>16.770299999999999</v>
-      </c>
-      <c r="F36">
-        <v>18.1492</v>
-      </c>
-      <c r="G36">
-        <v>26.290299999999998</v>
-      </c>
-      <c r="H36">
-        <v>62.319299999999998</v>
-      </c>
-      <c r="I36">
-        <v>146.46600000000001</v>
-      </c>
-      <c r="J36">
-        <v>279.71839999999997</v>
-      </c>
-      <c r="K36">
-        <v>544.2903</v>
-      </c>
-      <c r="P36" s="1">
-        <v>2048</v>
-      </c>
-      <c r="Q36">
-        <v>1.1778999999999999</v>
-      </c>
-      <c r="R36">
-        <v>1.6514</v>
-      </c>
-      <c r="S36">
-        <v>2.6373000000000002</v>
-      </c>
-      <c r="T36">
-        <v>4.5194999999999999</v>
-      </c>
-      <c r="U36">
-        <v>8.2566000000000006</v>
-      </c>
-      <c r="V36">
-        <v>16.091100000000001</v>
-      </c>
-      <c r="W36">
-        <v>32.732100000000003</v>
-      </c>
-      <c r="X36">
-        <v>66.802099999999996</v>
-      </c>
-      <c r="Y36">
-        <v>144.32550000000001</v>
-      </c>
-      <c r="Z36">
-        <v>288.84030000000001</v>
-      </c>
-    </row>
-    <row r="37" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="A37" s="1">
-        <v>4096</v>
-      </c>
-      <c r="P37" s="1">
-        <v>4096</v>
       </c>
     </row>
     <row r="38" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A38" s="1">
-        <v>8192</v>
+        <v>128</v>
+      </c>
+      <c r="B38">
+        <v>4.8661000000000003</v>
+      </c>
+      <c r="C38">
+        <v>4.8882000000000003</v>
+      </c>
+      <c r="D38">
+        <v>4.9641000000000002</v>
+      </c>
+      <c r="E38">
+        <v>5.1196000000000002</v>
+      </c>
+      <c r="F38">
+        <v>5.3280000000000003</v>
+      </c>
+      <c r="G38">
+        <v>5.6430999999999996</v>
+      </c>
+      <c r="H38">
+        <v>6.6346999999999996</v>
+      </c>
+      <c r="I38">
+        <v>9.8186999999999998</v>
+      </c>
+      <c r="J38">
+        <v>17.505199999999999</v>
+      </c>
+      <c r="K38">
+        <v>35.870100000000001</v>
+      </c>
+      <c r="L38">
+        <v>74.410600000000002</v>
       </c>
       <c r="P38" s="1">
-        <v>8192</v>
+        <v>128</v>
+      </c>
+      <c r="Q38" s="5">
+        <v>1.0468</v>
+      </c>
+      <c r="R38" s="5">
+        <v>1.4205000000000001</v>
+      </c>
+      <c r="S38" s="5">
+        <v>2.2820999999999998</v>
+      </c>
+      <c r="T38" s="5">
+        <v>3.9356</v>
+      </c>
+      <c r="U38" s="5">
+        <v>7.2767999999999997</v>
+      </c>
+      <c r="V38" s="5">
+        <v>13.8726</v>
+      </c>
+      <c r="W38" s="5">
+        <v>27.044</v>
+      </c>
+      <c r="X38" s="5">
+        <v>53.479799999999997</v>
+      </c>
+      <c r="Y38" s="5">
+        <v>106.0325</v>
+      </c>
+      <c r="Z38" s="5">
+        <v>211.68559999999999</v>
+      </c>
+      <c r="AA38" s="5">
+        <v>423.58030000000002</v>
       </c>
     </row>
     <row r="39" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A39" s="1">
-        <v>16384</v>
+        <v>256</v>
+      </c>
+      <c r="B39">
+        <v>5.7586000000000004</v>
+      </c>
+      <c r="C39">
+        <v>5.8208000000000002</v>
+      </c>
+      <c r="D39">
+        <v>5.9991000000000003</v>
+      </c>
+      <c r="E39">
+        <v>6.0632999999999999</v>
+      </c>
+      <c r="F39">
+        <v>6.3122999999999996</v>
+      </c>
+      <c r="G39">
+        <v>6.9637000000000002</v>
+      </c>
+      <c r="H39">
+        <v>9.3026</v>
+      </c>
+      <c r="I39">
+        <v>17.875800000000002</v>
+      </c>
+      <c r="J39">
+        <v>33.2316</v>
+      </c>
+      <c r="K39">
+        <v>69.363399999999999</v>
+      </c>
+      <c r="L39">
+        <v>145.5532</v>
       </c>
       <c r="P39" s="1">
-        <v>16384</v>
+        <v>256</v>
+      </c>
+      <c r="Q39" s="5">
+        <v>1.0177</v>
+      </c>
+      <c r="R39" s="5">
+        <v>1.4511000000000001</v>
+      </c>
+      <c r="S39" s="5">
+        <v>2.3130999999999999</v>
+      </c>
+      <c r="T39" s="5">
+        <v>3.9988000000000001</v>
+      </c>
+      <c r="U39" s="5">
+        <v>7.3720999999999997</v>
+      </c>
+      <c r="V39" s="5">
+        <v>14.101900000000001</v>
+      </c>
+      <c r="W39" s="5">
+        <v>27.500599999999999</v>
+      </c>
+      <c r="X39" s="5">
+        <v>54.220500000000001</v>
+      </c>
+      <c r="Y39" s="5">
+        <v>107.7698</v>
+      </c>
+      <c r="Z39" s="5">
+        <v>216.90170000000001</v>
+      </c>
+      <c r="AA39" s="5">
+        <v>442.46089999999998</v>
       </c>
     </row>
     <row r="40" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A40" s="1">
-        <v>32768</v>
+        <v>512</v>
+      </c>
+      <c r="B40">
+        <v>7.2171000000000003</v>
+      </c>
+      <c r="C40">
+        <v>7.2676999999999996</v>
+      </c>
+      <c r="D40">
+        <v>7.4058000000000002</v>
+      </c>
+      <c r="E40">
+        <v>7.6805000000000003</v>
+      </c>
+      <c r="F40">
+        <v>7.8780000000000001</v>
+      </c>
+      <c r="G40">
+        <v>9.2751999999999999</v>
+      </c>
+      <c r="H40">
+        <v>16.802900000000001</v>
+      </c>
+      <c r="I40">
+        <v>36.252899999999997</v>
+      </c>
+      <c r="J40">
+        <v>64.372200000000007</v>
+      </c>
+      <c r="K40">
+        <v>136.39420000000001</v>
+      </c>
+      <c r="L40">
+        <v>283.41660000000002</v>
       </c>
       <c r="P40" s="1">
-        <v>32768</v>
+        <v>512</v>
+      </c>
+      <c r="Q40" s="5">
+        <v>1.0412999999999999</v>
+      </c>
+      <c r="R40" s="5">
+        <v>1.4725999999999999</v>
+      </c>
+      <c r="S40" s="5">
+        <v>2.3595000000000002</v>
+      </c>
+      <c r="T40" s="5">
+        <v>4.0561999999999996</v>
+      </c>
+      <c r="U40" s="5">
+        <v>7.4831000000000003</v>
+      </c>
+      <c r="V40" s="5">
+        <v>14.2651</v>
+      </c>
+      <c r="W40" s="5">
+        <v>27.85</v>
+      </c>
+      <c r="X40" s="5">
+        <v>55.3964</v>
+      </c>
+      <c r="Y40" s="5">
+        <v>111.3929</v>
+      </c>
+      <c r="Z40" s="5">
+        <v>230.0112</v>
+      </c>
+      <c r="AA40" s="5">
+        <v>462.54090000000002</v>
       </c>
     </row>
     <row r="41" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A41" s="1">
-        <v>65536</v>
+        <v>1024</v>
+      </c>
+      <c r="B41">
+        <v>10.410600000000001</v>
+      </c>
+      <c r="C41">
+        <v>10.4734</v>
+      </c>
+      <c r="D41">
+        <v>10.660299999999999</v>
+      </c>
+      <c r="E41">
+        <v>10.9011</v>
+      </c>
+      <c r="F41">
+        <v>11.475300000000001</v>
+      </c>
+      <c r="G41">
+        <v>14.431100000000001</v>
+      </c>
+      <c r="H41">
+        <v>31.186900000000001</v>
+      </c>
+      <c r="I41">
+        <v>69.664000000000001</v>
+      </c>
+      <c r="J41">
+        <v>129.32140000000001</v>
+      </c>
+      <c r="K41">
+        <v>277.1678</v>
+      </c>
+      <c r="L41">
+        <v>570.41139999999996</v>
       </c>
       <c r="P41" s="1">
-        <v>65536</v>
+        <v>1024</v>
+      </c>
+      <c r="Q41" s="5">
+        <v>1.0940000000000001</v>
+      </c>
+      <c r="R41" s="5">
+        <v>1.5558000000000001</v>
+      </c>
+      <c r="S41" s="5">
+        <v>2.4428000000000001</v>
+      </c>
+      <c r="T41" s="5">
+        <v>4.2047999999999996</v>
+      </c>
+      <c r="U41" s="5">
+        <v>7.7328000000000001</v>
+      </c>
+      <c r="V41" s="5">
+        <v>14.768000000000001</v>
+      </c>
+      <c r="W41" s="5">
+        <v>29.1662</v>
+      </c>
+      <c r="X41" s="5">
+        <v>58.742699999999999</v>
+      </c>
+      <c r="Y41" s="5">
+        <v>124.4648</v>
+      </c>
+      <c r="Z41" s="5">
+        <v>249.95740000000001</v>
+      </c>
+      <c r="AA41" s="5">
+        <v>499.8057</v>
       </c>
     </row>
     <row r="42" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A42" s="1">
+        <v>2048</v>
+      </c>
+      <c r="B42">
+        <v>15.927099999999999</v>
+      </c>
+      <c r="C42">
+        <v>16.150400000000001</v>
+      </c>
+      <c r="D42">
+        <v>16.379100000000001</v>
+      </c>
+      <c r="E42">
+        <v>16.770299999999999</v>
+      </c>
+      <c r="F42">
+        <v>18.1492</v>
+      </c>
+      <c r="G42">
+        <v>26.290299999999998</v>
+      </c>
+      <c r="H42">
+        <v>62.319299999999998</v>
+      </c>
+      <c r="I42">
+        <v>146.46600000000001</v>
+      </c>
+      <c r="J42">
+        <v>279.71839999999997</v>
+      </c>
+      <c r="K42">
+        <v>544.2903</v>
+      </c>
+      <c r="L42">
+        <v>1137.6241</v>
+      </c>
+      <c r="P42" s="1">
+        <v>2048</v>
+      </c>
+      <c r="Q42" s="5">
+        <v>1.1778999999999999</v>
+      </c>
+      <c r="R42" s="5">
+        <v>1.6514</v>
+      </c>
+      <c r="S42" s="5">
+        <v>2.6373000000000002</v>
+      </c>
+      <c r="T42" s="5">
+        <v>4.5194999999999999</v>
+      </c>
+      <c r="U42" s="5">
+        <v>8.2566000000000006</v>
+      </c>
+      <c r="V42" s="5">
+        <v>16.091100000000001</v>
+      </c>
+      <c r="W42" s="5">
+        <v>32.732100000000003</v>
+      </c>
+      <c r="X42" s="5">
+        <v>66.802099999999996</v>
+      </c>
+      <c r="Y42" s="5">
+        <v>144.32550000000001</v>
+      </c>
+      <c r="Z42" s="5">
+        <v>288.84030000000001</v>
+      </c>
+      <c r="AA42" s="5">
+        <v>575.84690000000001</v>
+      </c>
+    </row>
+    <row r="43" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A43" s="1">
+        <v>4096</v>
+      </c>
+      <c r="B43">
+        <v>26.716799999999999</v>
+      </c>
+      <c r="C43">
+        <v>26.925699999999999</v>
+      </c>
+      <c r="D43">
+        <v>27.3613</v>
+      </c>
+      <c r="E43">
+        <v>28.200500000000002</v>
+      </c>
+      <c r="F43">
+        <v>31.1508</v>
+      </c>
+      <c r="G43">
+        <v>51.927799999999998</v>
+      </c>
+      <c r="H43">
+        <v>125.3653</v>
+      </c>
+      <c r="I43">
+        <v>289.57080000000002</v>
+      </c>
+      <c r="J43">
+        <v>571.70699999999999</v>
+      </c>
+      <c r="K43">
+        <v>1087.7055</v>
+      </c>
+      <c r="L43">
+        <v>2263.1806000000001</v>
+      </c>
+      <c r="P43" s="1">
+        <v>4096</v>
+      </c>
+      <c r="Q43" s="5">
+        <v>1.3636999999999999</v>
+      </c>
+      <c r="R43" s="5">
+        <v>1.9279999999999999</v>
+      </c>
+      <c r="S43" s="5">
+        <v>3.0097999999999998</v>
+      </c>
+      <c r="T43" s="5">
+        <v>5.1173000000000002</v>
+      </c>
+      <c r="U43" s="5">
+        <v>9.5327999999999999</v>
+      </c>
+      <c r="V43" s="5">
+        <v>19.046099999999999</v>
+      </c>
+      <c r="W43" s="5">
+        <v>44.939399999999999</v>
+      </c>
+      <c r="X43" s="5">
+        <v>90.937899999999999</v>
+      </c>
+      <c r="Y43" s="5">
+        <v>184.0744</v>
+      </c>
+      <c r="Z43" s="5">
+        <v>366.94189999999998</v>
+      </c>
+      <c r="AA43" s="5">
+        <v>733.64369999999997</v>
+      </c>
+    </row>
+    <row r="44" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A44" s="1">
+        <v>8192</v>
+      </c>
+      <c r="B44">
+        <v>47.486600000000003</v>
+      </c>
+      <c r="C44">
+        <v>48.109000000000002</v>
+      </c>
+      <c r="D44">
+        <v>49.145400000000002</v>
+      </c>
+      <c r="E44">
+        <v>51.232599999999998</v>
+      </c>
+      <c r="F44">
+        <v>57.158000000000001</v>
+      </c>
+      <c r="G44">
+        <v>105.2076</v>
+      </c>
+      <c r="H44">
+        <v>258.55720000000002</v>
+      </c>
+      <c r="I44">
+        <v>574.41340000000002</v>
+      </c>
+      <c r="J44">
+        <v>1135.2330999999999</v>
+      </c>
+      <c r="K44">
+        <v>2165.8512999999998</v>
+      </c>
+      <c r="L44">
+        <v>4494.2846</v>
+      </c>
+      <c r="P44" s="1">
+        <v>8192</v>
+      </c>
+      <c r="Q44" s="5">
+        <v>1.7479</v>
+      </c>
+      <c r="R44" s="5">
+        <v>2.4502999999999999</v>
+      </c>
+      <c r="S44" s="5">
+        <v>3.7723</v>
+      </c>
+      <c r="T44" s="5">
+        <v>6.6462000000000003</v>
+      </c>
+      <c r="U44" s="5">
+        <v>13.0991</v>
+      </c>
+      <c r="V44" s="5">
+        <v>31.841899999999999</v>
+      </c>
+      <c r="W44" s="5">
+        <v>64.973600000000005</v>
+      </c>
+      <c r="X44" s="5">
+        <v>130.28639999999999</v>
+      </c>
+      <c r="Y44" s="5">
+        <v>260.76620000000003</v>
+      </c>
+      <c r="Z44" s="5">
+        <v>523.41819999999996</v>
+      </c>
+      <c r="AA44" s="5">
+        <v>1039.8282999999999</v>
+      </c>
+    </row>
+    <row r="45" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A45" s="1">
+        <v>16384</v>
+      </c>
+      <c r="B45">
+        <v>90.826599999999999</v>
+      </c>
+      <c r="C45">
+        <v>92.826599999999999</v>
+      </c>
+      <c r="D45">
+        <v>94.920500000000004</v>
+      </c>
+      <c r="E45">
+        <v>98.846400000000003</v>
+      </c>
+      <c r="F45">
+        <v>109.645</v>
+      </c>
+      <c r="G45">
+        <v>218.7441</v>
+      </c>
+      <c r="H45">
+        <v>541.06410000000005</v>
+      </c>
+      <c r="I45">
+        <v>1270.5936999999999</v>
+      </c>
+      <c r="J45">
+        <v>2168.7869999999998</v>
+      </c>
+      <c r="K45">
+        <v>4351.6737999999996</v>
+      </c>
+      <c r="L45">
+        <v>9160.5710999999992</v>
+      </c>
+      <c r="P45" s="1">
+        <v>16384</v>
+      </c>
+      <c r="Q45" s="5">
+        <v>2.4849000000000001</v>
+      </c>
+      <c r="R45" s="5">
+        <v>3.4887000000000001</v>
+      </c>
+      <c r="S45" s="5">
+        <v>5.5635000000000003</v>
+      </c>
+      <c r="T45" s="5">
+        <v>10.6959</v>
+      </c>
+      <c r="U45" s="5">
+        <v>24.714500000000001</v>
+      </c>
+      <c r="V45" s="5">
+        <v>53.994100000000003</v>
+      </c>
+      <c r="W45" s="5">
+        <v>109.42740000000001</v>
+      </c>
+      <c r="X45" s="5">
+        <v>213.81890000000001</v>
+      </c>
+      <c r="Y45" s="5">
+        <v>405.49290000000002</v>
+      </c>
+      <c r="Z45" s="5">
+        <v>817.18439999999998</v>
+      </c>
+      <c r="AA45" s="5">
+        <v>1647.095</v>
+      </c>
+    </row>
+    <row r="46" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A46" s="1">
+        <v>32768</v>
+      </c>
+      <c r="B46">
+        <v>177.3638</v>
+      </c>
+      <c r="C46">
+        <v>179.9769</v>
+      </c>
+      <c r="D46">
+        <v>185.06729999999999</v>
+      </c>
+      <c r="E46">
+        <v>192.22900000000001</v>
+      </c>
+      <c r="F46">
+        <v>217.1919</v>
+      </c>
+      <c r="G46">
+        <v>382.9479</v>
+      </c>
+      <c r="H46">
+        <v>983.17079999999999</v>
+      </c>
+      <c r="I46">
+        <v>2170.7734999999998</v>
+      </c>
+      <c r="P46" s="1">
+        <v>32768</v>
+      </c>
+      <c r="Q46" s="5">
+        <v>4.0697000000000001</v>
+      </c>
+      <c r="R46" s="5">
+        <v>5.8958000000000004</v>
+      </c>
+      <c r="S46" s="5">
+        <v>9.8823000000000008</v>
+      </c>
+      <c r="T46" s="5">
+        <v>24.050699999999999</v>
+      </c>
+      <c r="U46" s="5">
+        <v>42.911200000000001</v>
+      </c>
+      <c r="V46" s="5">
+        <v>97.440700000000007</v>
+      </c>
+      <c r="W46" s="5">
+        <v>192.98330000000001</v>
+      </c>
+      <c r="X46" s="5">
+        <v>370.59309999999999</v>
+      </c>
+      <c r="Y46" s="5"/>
+      <c r="Z46" s="5"/>
+      <c r="AA46" s="5"/>
+    </row>
+    <row r="47" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A47" s="1">
+        <v>65536</v>
+      </c>
+      <c r="P47" s="1">
+        <v>65536</v>
+      </c>
+      <c r="Q47" s="5"/>
+      <c r="R47" s="5"/>
+      <c r="S47" s="5"/>
+      <c r="T47" s="5"/>
+      <c r="U47" s="5"/>
+      <c r="V47" s="5"/>
+      <c r="W47" s="5"/>
+      <c r="X47" s="5"/>
+      <c r="Y47" s="5"/>
+      <c r="Z47" s="5"/>
+      <c r="AA47" s="5"/>
+    </row>
+    <row r="48" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A48" s="1">
         <v>131072</v>
       </c>
-      <c r="P42" s="1">
+      <c r="P48" s="1">
         <v>131072</v>
+      </c>
+      <c r="Q48" s="5"/>
+      <c r="R48" s="5"/>
+      <c r="S48" s="5"/>
+      <c r="T48" s="5"/>
+      <c r="U48" s="5"/>
+      <c r="V48" s="5"/>
+      <c r="W48" s="5"/>
+      <c r="X48" s="5"/>
+      <c r="Y48" s="5"/>
+      <c r="Z48" s="5"/>
+      <c r="AA48" s="5"/>
+    </row>
+    <row r="50" spans="17:17" x14ac:dyDescent="0.2">
+      <c r="Q50" t="s">
+        <v>15</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="B3:H7">
+    <cfRule type="colorScale" priority="8">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B13:H17">
     <cfRule type="colorScale" priority="7">
       <colorScale>
         <cfvo type="min"/>
@@ -1504,7 +2189,19 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B13:H17">
+  <conditionalFormatting sqref="B23:H33 I23:L26 I27:J27">
+    <cfRule type="colorScale" priority="5">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B38:H39 B41:H42 B40:F40 I38:L38 I40:J40 B45">
     <cfRule type="colorScale" priority="6">
       <colorScale>
         <cfvo type="min"/>
@@ -1516,8 +2213,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B23:H27">
-    <cfRule type="colorScale" priority="4">
+  <conditionalFormatting sqref="B38:L48">
+    <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -1528,8 +2225,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B32:H33 B35:H36 B34:F34 I32:L32 I34:J34">
-    <cfRule type="colorScale" priority="5">
+  <conditionalFormatting sqref="Q38:AA45 Q46:X46">
+    <cfRule type="colorScale" priority="3">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -1540,8 +2237,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B32:L42">
-    <cfRule type="colorScale" priority="1">
+  <conditionalFormatting sqref="X38:Z38 Q38:W46">
+    <cfRule type="colorScale" priority="9">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -1552,20 +2249,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Q32:W36 X32:Z32">
-    <cfRule type="colorScale" priority="8">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="Q32:AA36">
-    <cfRule type="colorScale" priority="2">
+  <conditionalFormatting sqref="Q23:AA33">
+    <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>

</xml_diff>